<commit_message>
rename TRICALL to Triangulation add RefinePart, EdgeLengths add DepthFirstFindAllFaces
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C36BABD-02D0-4C4F-BBE9-2BC0494718C3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67A910B-E563-49A7-8387-B9664C86039D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="api calls" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>D</t>
   </si>
@@ -175,6 +175,18 @@
   <si>
     <t xml:space="preserve">Implement “Make Rectangular from samples” </t>
   </si>
+  <si>
+    <t>make interactive, solve last bugs</t>
+  </si>
+  <si>
+    <t>this should be easy</t>
+  </si>
+  <si>
+    <t>hours spent</t>
+  </si>
+  <si>
+    <t>Total hours spent so far</t>
+  </si>
 </sst>
 </file>
 
@@ -184,7 +196,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;€&quot;* #,##0_);_(&quot;€&quot;* \(#,##0\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,13 +227,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -332,8 +356,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -352,9 +377,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -691,22 +717,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="8" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -720,7 +746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -734,7 +760,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="E3" s="7" t="s">
         <v>3</v>
@@ -746,7 +772,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
@@ -757,7 +783,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -774,11 +800,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
@@ -799,8 +825,11 @@
       <c r="G7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -826,7 +855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -852,11 +881,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
@@ -878,11 +907,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="16" t="s">
         <v>38</v>
       </c>
       <c r="C11" t="s">
@@ -904,11 +933,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
@@ -930,7 +959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -956,11 +985,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C14" t="s">
@@ -982,11 +1011,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C15" t="s">
@@ -1008,11 +1037,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C16" t="s">
@@ -1034,11 +1063,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="16" t="s">
         <v>43</v>
       </c>
       <c r="C17" t="s">
@@ -1059,12 +1088,15 @@
       <c r="G17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C18" t="s">
@@ -1086,7 +1118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1112,7 +1144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1138,7 +1170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1164,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1174,7 +1206,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C23" s="11" t="s">
         <v>11</v>
       </c>
@@ -1192,7 +1224,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="13" t="s">
         <v>13</v>
       </c>
@@ -1211,11 +1243,62 @@
       </c>
       <c r="H24" s="5"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="16"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>26</v>
+      </c>
       <c r="C29" s="15"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36">
+        <f>SUM(B27:B34)</f>
+        <v>211</v>
+      </c>
+      <c r="C36">
+        <f>B36*135</f>
+        <v>28485</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
coorect triangle/CMakeLists.txt added test files FindFacesRecursive add HangingEdge test
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67A910B-E563-49A7-8387-B9664C86039D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF041FE-72EE-4136-8005-D80D3758145F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-525" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="begroting" sheetId="1" r:id="rId1"/>
-    <sheet name="api calls" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>D</t>
   </si>
@@ -89,12 +87,6 @@
     <t>Carniato, L.</t>
   </si>
   <si>
-    <t>FORTRAN subroutines</t>
-  </si>
-  <si>
-    <t>gridtonet</t>
-  </si>
-  <si>
     <t>Implement triangular mesh in polygon</t>
   </si>
   <si>
@@ -113,9 +105,6 @@
     <t>Part 4</t>
   </si>
   <si>
-    <t>API calls</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -153,9 +142,6 @@
   </si>
   <si>
     <t>Julian Hofer</t>
-  </si>
-  <si>
-    <t>mergenodes</t>
   </si>
   <si>
     <t>Add third party triangulation library (triangle.c)</t>
@@ -717,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,12 +729,12 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>2</v>
@@ -757,7 +743,7 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -769,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -802,13 +788,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <f>F7+G7</f>
@@ -826,18 +812,18 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D21" si="1">F8+G8</f>
@@ -857,13 +843,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
@@ -883,13 +869,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
@@ -909,13 +895,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
@@ -935,13 +921,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
@@ -961,13 +947,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
@@ -987,13 +973,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
@@ -1013,13 +999,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
@@ -1039,13 +1025,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
@@ -1065,13 +1051,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D17">
         <f t="shared" ref="D17" si="3">F17+G17</f>
@@ -1089,18 +1075,18 @@
         <v>4</v>
       </c>
       <c r="I17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
@@ -1120,13 +1106,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
@@ -1146,13 +1132,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
@@ -1172,13 +1158,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
@@ -1245,7 +1231,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B27">
         <v>22</v>
@@ -1287,16 +1273,16 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38">
         <f>SUM(B27:B34)</f>
         <v>211</v>
       </c>
-      <c r="C36">
-        <f>B36*135</f>
+      <c r="C38">
+        <f>B38*135</f>
         <v>28485</v>
       </c>
     </row>
@@ -1304,56 +1290,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="69.7109375" customWidth="1"/>
-    <col min="3" max="3" width="58.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
commit some pending changes
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF041FE-72EE-4136-8005-D80D3758145F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A351E8-A22C-4C6E-AD50-CEE63B37CE55}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-525" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="24270" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="begroting" sheetId="1" r:id="rId1"/>
@@ -703,9 +703,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -949,7 +949,7 @@
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C13" t="s">
@@ -1229,61 +1229,112 @@
       </c>
       <c r="H24" s="5"/>
     </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>42</v>
+      <c r="A27">
+        <v>2</v>
       </c>
       <c r="B27">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>26</v>
-      </c>
-      <c r="C29" s="15"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>13</v>
+      </c>
+      <c r="B36">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <f>14+19</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>43</v>
       </c>
-      <c r="B38">
-        <f>SUM(B27:B34)</f>
-        <v>211</v>
-      </c>
-      <c r="C38">
-        <f>B38*135</f>
-        <v>28485</v>
+      <c r="B42">
+        <f>SUM(B27:B40)</f>
+        <v>288</v>
+      </c>
+      <c r="C42">
+        <f>B42*135</f>
+        <v>38880</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added: ggeo_vertices_in_polygons ggeo_insert_edge ggeo_insert_node ggeo_delete_node ggeo_offsetted_polygon
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A351E8-A22C-4C6E-AD50-CEE63B37CE55}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FE8884-35BF-45B4-85C4-621F974656DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="24270" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="24270" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="begroting" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>D</t>
   </si>
@@ -172,6 +173,21 @@
   </si>
   <si>
     <t>Total hours spent so far</t>
+  </si>
+  <si>
+    <t>ctrl + x</t>
+  </si>
+  <si>
+    <t>interactor instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shift + c </t>
+  </si>
+  <si>
+    <t>polygong offset</t>
+  </si>
+  <si>
+    <t>use buffers for nodes and edges</t>
   </si>
 </sst>
 </file>
@@ -705,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +861,7 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C9" t="s">
@@ -1134,7 +1150,7 @@
       <c r="A20" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C20" t="s">
@@ -1160,7 +1176,7 @@
       <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C21" t="s">
@@ -1341,4 +1357,41 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7E1334-7D01-4EA0-B6BD-E48974BADECC}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add forward declarations start with mesh refinement
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FE8884-35BF-45B4-85C4-621F974656DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B484B3E8-6047-4DE4-8B67-F6E81C019873}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="24270" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-525" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="begroting" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>D</t>
   </si>
@@ -188,6 +188,15 @@
   </si>
   <si>
     <t>use buffers for nodes and edges</t>
+  </si>
+  <si>
+    <t>generate curvilinear grid from spline: spli api, create cpp file</t>
+  </si>
+  <si>
+    <t>dtmax</t>
+  </si>
+  <si>
+    <t>dx</t>
   </si>
 </sst>
 </file>
@@ -396,6 +405,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{991535EB-D66D-4CD8-B174-ED7770939E96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4886325" y="28575"/>
+          <a:ext cx="7896225" cy="1781175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1361,10 +1436,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7E1334-7D01-4EA0-B6BD-E48974BADECC}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,8 +1465,31 @@
         <v>48</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <f>B6/SQRT(9.81)</f>
+        <v>0.63855085681410095</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
polygonCache in landboundaries resized where used averaging added continued with refine based on sample
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B484B3E8-6047-4DE4-8B67-F6E81C019873}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A865C0-4CBF-428E-9CDA-7663BF74D57A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-525" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="24270" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="begroting" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>D</t>
   </si>
@@ -198,6 +198,12 @@
   <si>
     <t>dx</t>
   </si>
+  <si>
+    <t>week number</t>
+  </si>
+  <si>
+    <t>budget</t>
+  </si>
 </sst>
 </file>
 
@@ -207,7 +213,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;€&quot;* #,##0_);_(&quot;€&quot;* \(#,##0\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +251,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +269,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -367,11 +385,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -389,9 +408,11 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -796,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1220,7 @@
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C19" t="s">
@@ -1322,6 +1343,9 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1415,17 +1439,35 @@
         <v>33</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
       <c r="B42">
         <f>SUM(B27:B40)</f>
-        <v>288</v>
+        <v>322</v>
       </c>
       <c r="C42">
         <f>B42*135</f>
-        <v>38880</v>
+        <v>43470</v>
       </c>
     </row>
   </sheetData>
@@ -1438,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7E1334-7D01-4EA0-B6BD-E48974BADECC}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,7 +1517,7 @@
         <v>51</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1484,7 +1526,7 @@
       </c>
       <c r="B7">
         <f>B6/SQRT(9.81)</f>
-        <v>0.63855085681410095</v>
+        <v>1.5963771420352522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added latest grid editor version
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A865C0-4CBF-428E-9CDA-7663BF74D57A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9692D79-07F4-4DEC-A6B7-22487C94D8A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="24270" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="24270" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="begroting" sheetId="1" r:id="rId1"/>
@@ -213,7 +213,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;€&quot;* #,##0_);_(&quot;€&quot;* \(#,##0\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,15 +251,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,11 +262,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -385,12 +373,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -408,11 +395,9 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -815,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,7 +1205,7 @@
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C19" t="s">
@@ -1451,23 +1436,34 @@
       <c r="A39">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="B39">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>17</v>
+      </c>
+      <c r="B40">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>43</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <f>SUM(B27:B40)</f>
-        <v>322</v>
-      </c>
-      <c r="C42">
-        <f>B42*135</f>
-        <v>43470</v>
+        <v>382</v>
+      </c>
+      <c r="C43">
+        <f>B43*135</f>
+        <v>51570</v>
       </c>
     </row>
   </sheetData>
@@ -1480,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7E1334-7D01-4EA0-B6BD-E48974BADECC}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
in ggeo_set_state re-activate spherical coordinates add helper MakeRectangularMeshForTesting method for making rectangular grids in unit test LandBoundaryTest.cpp add FourByFourWithFourSamplesSpherical test
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9692D79-07F4-4DEC-A6B7-22487C94D8A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF67F68-2303-4D6E-82DA-C2C4F389FB73}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="24270" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1445,7 +1445,7 @@
         <v>17</v>
       </c>
       <c r="B40">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1459,11 +1459,11 @@
       </c>
       <c r="B43">
         <f>SUM(B27:B40)</f>
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="C43">
         <f>B43*135</f>
-        <v>51570</v>
+        <v>51975</v>
       </c>
     </row>
   </sheetData>
@@ -1474,15 +1474,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7E1334-7D01-4EA0-B6BD-E48974BADECC}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1498,31 +1498,45 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
       <c r="B7">
         <f>B6/SQRT(9.81)</f>
         <v>1.5963771420352522</v>
+      </c>
+      <c r="C7">
+        <f>C6/SQRT(9.81)</f>
+        <v>0.95782628522115132</v>
+      </c>
+      <c r="D7">
+        <f>D6/SQRT(9.81)</f>
+        <v>0.31927542840705048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>